<commit_message>
Fixed autocomplete on page StatisticPerWell
</commit_message>
<xml_diff>
--- a/LOVA.API/wwwroot/Upload/Lottingmedlemmar_27-oktober.xlsx
+++ b/LOVA.API/wwwroot/Upload/Lottingmedlemmar_27-oktober.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/149100657e615279/Löttingelund/Hemsida/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{E85F8F80-275A-445D-BFC9-E814AF8A20D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7D337FC2-6D8C-448C-BA7F-86D0AC3A689E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{E85F8F80-275A-445D-BFC9-E814AF8A20D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E04DA2D-B7EB-4637-8704-75B504763EAE}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4672,8 +4672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4691,7 +4691,7 @@
     <col min="12" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>

</xml_diff>